<commit_message>
fix: fix to Geo2.xlsx for Palisaden
</commit_message>
<xml_diff>
--- a/test_data/palisaden/Geo2.xlsx
+++ b/test_data/palisaden/Geo2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://treteknisk-my.sharepoint.com/personal/dpa_treteknisk_no/Documents/Dokumenter/Dev/pyOMA2/src/pyoma2/test_data/palisaden/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://treteknisk-my.sharepoint.com/personal/dpa_treteknisk_no/Documents/Dokumenter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="11_AD4D5CB4E552A5DACE1C6441785E53185BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E1FFB82-7001-401A-BFD5-BC01E98AF214}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{475B37BA-43BC-4ACE-A33F-1C8E4CB919AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="775" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33090" yWindow="3195" windowWidth="21600" windowHeight="12645" tabRatio="775" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="11" r:id="rId1"/>
@@ -156,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,6 +165,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -556,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5482AEB-1D8E-486C-90C8-0466A2CBFF04}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
@@ -753,7 +756,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D7"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,10 +870,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDBCE1F-47DB-4811-BB35-0E0205CD2B40}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +882,7 @@
     <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -893,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -901,32 +904,32 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>19</v>
@@ -935,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -949,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -963,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -976,6 +979,9 @@
       <c r="D7" s="2">
         <v>0</v>
       </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: Geo2 file for palisaden
</commit_message>
<xml_diff>
--- a/test_data/palisaden/Geo2.xlsx
+++ b/test_data/palisaden/Geo2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://treteknisk-my.sharepoint.com/personal/dpa_treteknisk_no/Documents/Dokumenter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{475B37BA-43BC-4ACE-A33F-1C8E4CB919AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{475B37BA-43BC-4ACE-A33F-1C8E4CB919AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CE5F1DC-0CA2-4A98-9526-80C1CC46FC55}"/>
   <bookViews>
-    <workbookView xWindow="33090" yWindow="3195" windowWidth="21600" windowHeight="12645" tabRatio="775" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4785" yWindow="3150" windowWidth="21600" windowHeight="12645" tabRatio="775" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="11" r:id="rId1"/>
@@ -755,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A15A84-EA7B-425C-9E23-D6961CCE0DF3}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDBCE1F-47DB-4811-BB35-0E0205CD2B40}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +904,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -915,10 +915,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -929,7 +929,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>19</v>

</xml_diff>